<commit_message>
adds reasoning count limit
</commit_message>
<xml_diff>
--- a/main/results/jdk1_1.xlsx
+++ b/main/results/jdk1_1.xlsx
@@ -492,19 +492,19 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>74.02</v>
+        <v>89.42</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The applicant has shown strong skills in ReactJS, Django, Python, JavaScript, and computer vision which aligns with the company's requirement for MongoDB, ReactJS, JavaScript, Web Development, and NodeJS. The applicant's experience in developing web applications using ReactJS and Django showcases their ability to work with technologies similar to those required for the internship. Additionally, the applicant has demonstrated proficiency in computer vision and image processing, indicating their capability to work on tasks related to web/mobile application development. However, the applicant lacks explicit experience with MongoDB, which is a required skill for the internship. While the applicant's skills are commendable, the absence of explicit MongoDB experience may impact their readiness for the specific tasks related to MongoDB in the internship.</t>
+          <t>The applicant has a good understanding of web development technologies such as ReactJS, NodeJS, ExpressJS, and WebRTC, which are essential for the mentioned job role. The applicant has also worked on relevant projects showcasing skills in Flutter, Dart, Firebase, and Docker, demonstrating an ability to work with modern web and mobile technologies. While the applicant may not have direct experience with MongoDB, the applicant's strong technical skills and adaptability make them well-suited to quickly learn and apply this skill in the given role.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>応募者はReactJS、Django、Python、JavaScript、およびコンピュータビジョンのスキルを示し、これは企業が求めるMongoDB、ReactJS、JavaScript、Web開発、およびNodeJSに合致しています。応募者のReactJSとDjangoを使用したウェブアプリケーション開発の経験は、インターンシップで必要な技術と類似したテクノロジーに対する能力を示しています。さらに、応募者はコンピュータビジョンと画像処理の習熟を示し、それはWeb /モバイルアプリケーション開発に関連するタスクに取り組む能力を示しています。ただし、応募者はMongoDBの明確な経験を持っていないため、特定のMongoDB関連のタスクに対する準備状況に影響を与える可能性があります。</t>
+          <t>応募者は、ReactJS、NodeJS、ExpressJS、およびWebRTCなどのWeb開発技術について良い理解を持っており、これらは述べられた職務にとって不可欠です。応募者はまた、Flutter、Dart、Firebase、およびDockerのスキルを示す関連するプロジェクトで働いており、最新のWebおよびモバイル技術を扱う能力を示しています。応募者は直接的なMongoDBの経験を持っていないかもしれませんが、強力な技術スキルと適応性があり、与えられた役割で迅速にこのスキルを学び適用する能力を持っています。</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -512,17 +512,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>The applicant has shown a strong willingness to learn, adapt, and collaborate, as evidenced by their proactive approach to self-improvement, seeking feedback, and participating in workshops and online courses. The applicant's expressed interest in learning from Japanese work culture and their appreciation for values like hard work, punctuality, and dedication align well with the company's cultural ethos. Their positive attitude and commitment to holistic personal development make them a suitable candidate for the internship.</t>
+          <t>The applicant has demonstrated a strong willingness to adapt to new cultures, as well as a keen interest in Japan's work culture and language. Additionally, the applicant has showcased good teamwork and communication skills, along with a problem-solving approach. The applicant's future career plans align with the company's focus on AI/ML and backend development, indicating a good fit for the company's goals.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>応募者は、自己改善への積極的アプローチ、フィードバックの収集、ワークショップやオンラインコースへの積極的な参加など、学習意欲、適応能力、協力に対する強い意思を示しています。応募者が日本の労働文化から学びたいという意欲と、努力、時間厳守、献身といった価値観に対する感謝の表明は、企業の文化理念とよく合っています。彼らの前向きな姿勢と包括的な個人的成長へのコミットメントは、彼らをインターンシップに適した候補者にしています。</t>
+          <t>応募者は新しい文化に適応する意欲が強く、日本の労働文化や言語に強い興味を示しています。さらに、応募者は良いチームワークとコミュニケーションスキル、問題解決のアプローチを披露しています。応募者の将来のキャリアプランは、AI / MLおよびバックエンド開発に焦点を当てている会社の目標と一致しており、会社の目標に適しています。</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Shubh</t>
+          <t>Suk</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -543,37 +543,19 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>89.42</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>The applicant has a high level of expertise in web development, as evidenced by their projects involving Flutter, Dart, Firebase, WebRTC, and Socket.IO. Although the projects do not directly involve the MERN stack, they showcase the applicant's proficiency in relevant technologies including ReactJS, NodeJS, and ExpressJS, which are crucial for the role. The candidate's diverse skill set and experience in developing web and mobile applications make them a suitable candidate for the SDE Intern position.</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>応募者はFlutter、Dart、Firebase、WebRTC、およびSocket.IOを使用したプロジェクトを通じてWeb開発の高度な専門知識を持っています。プロジェクトは直接的にMERNスタックを使用していませんが、ReactJS、NodeJS、ExpressJSなどの関連技術の習熟度を示しており、それはこの役割にとって重要です。応募者の多様なスキルセットとWebおよびモバイルアプリケーションの開発経験は、SDEインターンのポジションに適した候補者としています。</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>The candidate has shown a strong willingness to adapt to new cultures and expressed a keen interest in being a part of Japan's work culture. Additionally, the applicant demonstrated the ability to work in a team and acknowledged the importance of open communication and problem-solving. However, there is a slight concern about the applicant's preference not to work alone and the time taken to acquire new skills, which may require support and encouragement in adapting to a new work environment in Japan.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>応募者は新しい文化に適応する意欲を示し、日本の労働文化の一部になりたいという強い関心を表明しました。加えて、応募者はチームで働く能力を示し、オープンなコミュニケーションと問題解決の重要性を認識しました。ただし、応募者が単独での作業を好まず、新しいスキルを獲得する時間がかかることには少し懸念があります。これは、日本の新しい労働環境に適応するためにサポートと励ましが必要とされるかもしれません。</t>
-        </is>
-      </c>
+        <v>82.91</v>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Suk</t>
+          <t>Se</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -599,29 +581,11 @@
       <c r="B4" t="n">
         <v>77.25</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>The applicant has shown expertise in Python, PyTorch, TensorFlow, Keras, and Django Rest Framework which are relevant to back-end development. However, the required skills for this job position specifically involve MongoDB, ReactJS, JavaScript, Web Development, and NodeJS, which are not fully reflected in the applicant's projects and skills. While the applicant's experience in web development using Django Rest Framework and ReactJS demonstrates potential, there is a gap in direct experience with the technologies mentioned in the job description. Although the applicant's projects exhibit strong technical skills, they may not entirely align with the specific requirements of this position.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>応募者は、バックエンド開発に関連するPython、PyTorch、TensorFlow、Keras、およびDjango Rest Frameworkの専門知識を示しています。ただし、この仕事のために必要なスキルは、MongoDB、ReactJS、JavaScript、Web開発、およびNodeJSであり、これらは応募者のプロジェクトとスキルに完全に反映されていません。Django Rest FrameworkとReactJSを使用したWeb開発の経験が応募者の潜在能力を示していますが、求人の要件で具体的に言及されている技術と直接的な経験にはギャップがあります。応募者のプロジェクトは強力な技術スキルを示していますが、それらがこのポジションの具体的な要件と完全に一致しない可能性があります。</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>The applicant has demonstrated adaptability and a willingness to embrace new cultures, as evident from the answers provided. Their acknowledgment of the tight project deadline and the subsequent adoption of a collaborative problem-solving approach demonstrates excellent teamwork and problem-solving skills. Additionally, the applicant's interest in learning a new language while working in Japan exhibits openness to cultural immersion. However, the mention of relying on teamwork and the preference not to work alone could indicate a need for further development in individual problem-solving abilities, which might be essential in a remote working environment.</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>応募者は、提供された回答から明らかなように、適応性を示し、新しい文化を受け入れる意思があります。プロジェクトの厳しい締め切りやそれに続く共同問題解決アプローチの採用によって、優れたチームワークと問題解決能力が示されています。加えて、日本で働きながら新しい言語を学ぶことに興味を持つことは、文化的浸透への開放性を示しています。ただし、チームワークへの依存の言及や単独での作業を好まないことは、個人の問題解決能力のさらなる向上が必要である可能性を示しており、これはリモートワーキング環境で重要となるかもしれません。</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
           <t>Ya</t>
@@ -645,37 +609,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>82.91</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>The applicant has experience working on web development projects using JavaScript, HTML, and CSS, which are required skills for the job. The 'Video Conferencing Project' shows the applicant's ability to work on a project involving various functionalities like messaging, file sharing, and video/audio calls, indicating a good understanding of web/mobile applications. Additionally, the 'Alcheringa Pass Portal' project demonstrates the applicant's proficiency in creating websites for events. Although the projects do not specifically mention the use of MongoDB or NodeJS, the applicant's skills in JavaScript and web development are transferable to working with these technologies. Overall, the applicant's projects align well with the responsibilities of the SDE Intern position, and they exhibit the necessary skills for the job.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>応募者はJavaScript、HTML、CSSを使用したWeb開発プロジェクトの経験があり、それが求められるスキルである。『Video Conferencing Project』は、メッセージング、ファイル共有、およびビデオ/オーディオ通話などのさまざまな機能を持つプロジェクトに取り組んだ経験を示しており、Web/モバイルアプリケーションについての理解が深いことを示している。また、『Alcheringa Pass Portal』プロジェクトは、イベントのためのウェブサイトを作成する能力を示している。このプロジェクトにはMongoDBやNodeJSの具体的な使用が明記されていないが、応募者のJavaScriptおよびWeb開発のスキルは、これらの技術との作業にも適応可能である。全体的に、応募者のプロジェクトはSDE Internの職務内容とよく一致しており、求められるスキルを備えている。</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>The applicant has demonstrated strong communication skills by expressing a clear interest in Japan and its work culture. The willingness to adapt to a new culture and learn a new language, along with the desire to work on cutting-edge AI/ML technologies, showcases adaptability and problem-solving abilities. Additionally, the applicant's acknowledgment of the need to improve and learn new skills, along with the collaborative approach to problem-solving, reflects good teamwork and time management. Overall, the applicant's responses align with the company's soft skill requirements and demonstrate a positive attitude towards working in Japan.</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>応募者は日本とその労働文化に対する明確な興味を示すことで、強力なコミュニケーションスキルを発揮している。新しい文化に適応し、新しい言語を学ぶ意欲、そして最先端のAI / ML技術に取り組む意欲は、適応力と問題解決能力を示している。さらに、スキル向上と新しいスキルの習得の必要性を認識し、問題解決への協力的なアプローチから、良いチームワークとタイムマネジメントを反映している。全体的に、応募者の回答は会社のソフトスキル要件と一致しており、日本での勤務に対する肯定的な姿勢を示している。</t>
-        </is>
-      </c>
+        <v>74.02</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Se</t>
+          <t>Shubh</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">

</xml_diff>